<commit_message>
can update all implemented types
</commit_message>
<xml_diff>
--- a/data-files/OutExcel1.xlsx
+++ b/data-files/OutExcel1.xlsx
@@ -438,13 +438,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgriq5jx-hhmr</v>
+        <v>lgs4l68f-wupv</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T05:06:43.485Z</v>
+        <v>2023-04-22T15:18:42.639Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgriq5jx</v>
+        <v>lgs4l68f</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -467,13 +467,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgriq5jx-hpwc</v>
+        <v>lgs4l68g-jlfh</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T05:06:43.485Z</v>
+        <v>2023-04-22T15:18:42.640Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgriq5jx</v>
+        <v>lgs4l68g</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -496,13 +496,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgriq5jx-lvss</v>
+        <v>lgs4l68g-095d</v>
       </c>
       <c r="B4" t="str">
-        <v>2023-04-22T05:06:43.485Z</v>
+        <v>2023-04-22T15:18:42.640Z</v>
       </c>
       <c r="C4" t="str">
-        <v>lgriq5jx</v>
+        <v>lgs4l68g</v>
       </c>
       <c r="D4" t="str">
         <v>FALSE</v>
@@ -532,7 +532,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -571,19 +571,16 @@
       <c r="K1" t="str">
         <v>_rollup</v>
       </c>
-      <c r="L1" t="str">
-        <v>_format</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgriq5jx-c0dl</v>
+        <v>lgs4l68g-0qsw</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T05:06:43.485Z</v>
+        <v>2023-04-22T15:18:42.640Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgriq5jx</v>
+        <v>lgs4l68g</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -592,7 +589,7 @@
         <v>05a8</v>
       </c>
       <c r="F2" t="str">
-        <v>0ezi</v>
+        <v>ats6</v>
       </c>
       <c r="G2" t="str">
         <v>Free Item</v>
@@ -609,19 +606,16 @@
       <c r="K2" t="str">
         <v>COUNT</v>
       </c>
-      <c r="L2" t="str">
-        <v>TEXT</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgriq5jx-0g4b</v>
+        <v>lgs4l68g-mj7s</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T05:06:43.485Z</v>
+        <v>2023-04-22T15:18:42.640Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgriq5jx</v>
+        <v>lgs4l68g</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -647,19 +641,16 @@
       <c r="K3" t="str">
         <v>COUNT</v>
       </c>
-      <c r="L3" t="str">
-        <v>TEXT</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgriq5jx-7geo</v>
+        <v>lgs4l68g-hvoj</v>
       </c>
       <c r="B4" t="str">
-        <v>2023-04-22T05:06:43.485Z</v>
+        <v>2023-04-22T15:18:42.640Z</v>
       </c>
       <c r="C4" t="str">
-        <v>lgriq5jx</v>
+        <v>lgs4l68g</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -677,7 +668,7 @@
         <v>👍</v>
       </c>
       <c r="I4" t="str">
-        <v>Set a description</v>
+        <v>Orig desc</v>
       </c>
       <c r="J4" t="str">
         <v>BOOL</v>
@@ -685,13 +676,10 @@
       <c r="K4" t="str">
         <v>COUNT</v>
       </c>
-      <c r="L4" t="str">
-        <v>TEXT</v>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K4"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -731,13 +719,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgriq5jx-dcxf</v>
+        <v>lgs4l68g-0f7a</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T05:06:43.485Z</v>
+        <v>2023-04-22T15:18:42.640Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgriq5jx</v>
+        <v>lgs4l68g</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -749,21 +737,21 @@
         <v>lgricx7k-08al</v>
       </c>
       <c r="G2" t="str">
-        <v>2023-04-22T00</v>
+        <v>2023-04-22T06</v>
       </c>
       <c r="H2" t="str">
-        <v/>
+        <v>Orig note</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgriq5kb-qv7e</v>
+        <v>lgs4l68h-13pq</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T05:06:43.499Z</v>
+        <v>2023-04-22T15:18:42.641Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgriq5kb</v>
+        <v>lgs4l68h</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -772,10 +760,10 @@
         <v>0m7w</v>
       </c>
       <c r="F3" t="str">
-        <v>lgriq5kb-014e</v>
+        <v>lgs4l68s-gttg</v>
       </c>
       <c r="G3" t="str">
-        <v>2023-04-22T00:06:43</v>
+        <v>2023-04-22T10:18:42</v>
       </c>
       <c r="H3" t="str">
         <v/>
@@ -823,13 +811,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgriq5kb-dyjl</v>
+        <v>lgs4l68h-w50n</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T05:06:43.499Z</v>
+        <v>2023-04-22T15:18:42.641Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgriq5kb</v>
+        <v>lgs4l68h</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -849,13 +837,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgriq5kb-3314</v>
+        <v>lgs4l68h-1bns</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T05:06:43.499Z</v>
+        <v>2023-04-22T15:18:42.641Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgriq5kb</v>
+        <v>lgs4l68h</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
can indirectly update EntryPoints and PointDefs
</commit_message>
<xml_diff>
--- a/data-files/OutExcel1.xlsx
+++ b/data-files/OutExcel1.xlsx
@@ -438,13 +438,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs4l68f-wupv</v>
+        <v>lgs5e3pj-elk6</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T15:18:42.639Z</v>
+        <v>2023-04-22T15:41:12.391Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs4l68f</v>
+        <v>lgs5e3pj</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -467,13 +467,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs4l68g-jlfh</v>
+        <v>lgs5e3pj-6tewf</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T15:18:42.640Z</v>
+        <v>2023-04-22T15:41:12.391Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs4l68g</v>
+        <v>lgs5e3pj</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -496,13 +496,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgs4l68g-095d</v>
+        <v>lgs5e3pj-1ve7</v>
       </c>
       <c r="B4" t="str">
-        <v>2023-04-22T15:18:42.640Z</v>
+        <v>2023-04-22T15:41:12.391Z</v>
       </c>
       <c r="C4" t="str">
-        <v>lgs4l68g</v>
+        <v>lgs5e3pj</v>
       </c>
       <c r="D4" t="str">
         <v>FALSE</v>
@@ -574,13 +574,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs4l68g-0qsw</v>
+        <v>lgs5e3pk-0cjl</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T15:18:42.640Z</v>
+        <v>2023-04-22T15:41:12.392Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs4l68g</v>
+        <v>lgs5e3pk</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -589,7 +589,7 @@
         <v>05a8</v>
       </c>
       <c r="F2" t="str">
-        <v>ats6</v>
+        <v>0eze</v>
       </c>
       <c r="G2" t="str">
         <v>Free Item</v>
@@ -609,13 +609,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs4l68g-mj7s</v>
+        <v>lgs5e3pk-d89q</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T15:18:42.640Z</v>
+        <v>2023-04-22T15:41:12.392Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs4l68g</v>
+        <v>lgs5e3pk</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -644,13 +644,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgs4l68g-hvoj</v>
+        <v>lgs5e3pk-0kt2</v>
       </c>
       <c r="B4" t="str">
-        <v>2023-04-22T15:18:42.640Z</v>
+        <v>2023-04-22T15:41:12.392Z</v>
       </c>
       <c r="C4" t="str">
-        <v>lgs4l68g</v>
+        <v>lgs5e3pk</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -719,13 +719,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs4l68g-0f7a</v>
+        <v>lgs5e3pk-ust9</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T15:18:42.640Z</v>
+        <v>2023-04-22T15:41:12.392Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs4l68g</v>
+        <v>lgs5e3pk</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -745,13 +745,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs4l68h-13pq</v>
+        <v>lgs5e3pk-euus</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T15:18:42.641Z</v>
+        <v>2023-04-22T15:41:12.392Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs4l68h</v>
+        <v>lgs5e3pk</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -760,10 +760,10 @@
         <v>0m7w</v>
       </c>
       <c r="F3" t="str">
-        <v>lgs4l68s-gttg</v>
+        <v>lgs5e3pv-5ph5n</v>
       </c>
       <c r="G3" t="str">
-        <v>2023-04-22T10:18:42</v>
+        <v>2023-04-22T10:41:12</v>
       </c>
       <c r="H3" t="str">
         <v/>
@@ -811,13 +811,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs4l68h-w50n</v>
+        <v>lgs5e3pk-00bg</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T15:18:42.641Z</v>
+        <v>2023-04-22T15:41:12.392Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs4l68h</v>
+        <v>lgs5e3pk</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -837,13 +837,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs4l68h-1bns</v>
+        <v>lgs5e3pk-5gq2</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T15:18:42.641Z</v>
+        <v>2023-04-22T15:41:12.392Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs4l68h</v>
+        <v>lgs5e3pk</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
all fundamental components work?
</commit_message>
<xml_diff>
--- a/data-files/OutExcel1.xlsx
+++ b/data-files/OutExcel1.xlsx
@@ -438,13 +438,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs5e3pj-elk6</v>
+        <v>lgs8j8fo-06px</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T15:41:12.391Z</v>
+        <v>2023-04-22T17:09:10.644Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs5e3pj</v>
+        <v>lgs8j8fo</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -467,13 +467,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs5e3pj-6tewf</v>
+        <v>lgs8j8fo-0oj7</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T15:41:12.391Z</v>
+        <v>2023-04-22T17:09:10.644Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs5e3pj</v>
+        <v>lgs8j8fo</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -496,13 +496,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgs5e3pj-1ve7</v>
+        <v>lgs8j8fo-03ay</v>
       </c>
       <c r="B4" t="str">
-        <v>2023-04-22T15:41:12.391Z</v>
+        <v>2023-04-22T17:09:10.644Z</v>
       </c>
       <c r="C4" t="str">
-        <v>lgs5e3pj</v>
+        <v>lgs8j8fo</v>
       </c>
       <c r="D4" t="str">
         <v>FALSE</v>
@@ -532,7 +532,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -574,69 +574,69 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs5e3pk-0cjl</v>
+        <v>lgs8j8fo-pjps</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T15:41:12.392Z</v>
+        <v>2023-04-22T17:09:10.644Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs5e3pk</v>
+        <v>lgs8j8fo</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="str">
-        <v>05a8</v>
+        <v>0m7w</v>
       </c>
       <c r="F2" t="str">
-        <v>0eze</v>
+        <v>8esq</v>
       </c>
       <c r="G2" t="str">
-        <v>Free Item</v>
+        <v>Select Test</v>
       </c>
       <c r="H2" t="str">
-        <v>🆓</v>
+        <v>⛏️</v>
       </c>
       <c r="I2" t="str">
-        <v>Set a description</v>
+        <v>For testing selects</v>
       </c>
       <c r="J2" t="str">
-        <v>TEXT</v>
+        <v>SELECT</v>
       </c>
       <c r="K2" t="str">
-        <v>COUNT</v>
+        <v>COUNTOFEACH</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs5e3pk-d89q</v>
+        <v>lgs8j8fo-27z6i</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T15:41:12.392Z</v>
+        <v>2023-04-22T17:09:10.644Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs5e3pk</v>
+        <v>lgs8j8fo</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="str">
-        <v>ay7l</v>
+        <v>05a8</v>
       </c>
       <c r="F3" t="str">
-        <v>0pc6</v>
+        <v>1vb5</v>
       </c>
       <c r="G3" t="str">
-        <v>Numeric Thing</v>
+        <v>Free Item</v>
       </c>
       <c r="H3" t="str">
-        <v>#️⃣</v>
+        <v>🆓</v>
       </c>
       <c r="I3" t="str">
         <v>Set a description</v>
       </c>
       <c r="J3" t="str">
-        <v>NUM</v>
+        <v>TEXT</v>
       </c>
       <c r="K3" t="str">
         <v>COUNT</v>
@@ -644,13 +644,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgs5e3pk-0kt2</v>
+        <v>lgs8j8fo-62i6</v>
       </c>
       <c r="B4" t="str">
-        <v>2023-04-22T15:41:12.392Z</v>
+        <v>2023-04-22T17:09:10.644Z</v>
       </c>
       <c r="C4" t="str">
-        <v>lgs5e3pk</v>
+        <v>lgs8j8fo</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -659,27 +659,62 @@
         <v>ay7l</v>
       </c>
       <c r="F4" t="str">
+        <v>0pc6</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Numeric Thing</v>
+      </c>
+      <c r="H4" t="str">
+        <v>#️⃣</v>
+      </c>
+      <c r="I4" t="str">
+        <v>Set a description</v>
+      </c>
+      <c r="J4" t="str">
+        <v>NUM</v>
+      </c>
+      <c r="K4" t="str">
+        <v>AVERAGE</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>lgs8j8fo-nljl</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2023-04-22T17:09:10.644Z</v>
+      </c>
+      <c r="C5" t="str">
+        <v>lgs8j8fo</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
+        <v>ay7l</v>
+      </c>
+      <c r="F5" t="str">
         <v>0tb7</v>
       </c>
-      <c r="G4" t="str">
+      <c r="G5" t="str">
         <v>Boolean Thing</v>
       </c>
-      <c r="H4" t="str">
+      <c r="H5" t="str">
         <v>👍</v>
       </c>
-      <c r="I4" t="str">
+      <c r="I5" t="str">
         <v>Orig desc</v>
       </c>
-      <c r="J4" t="str">
+      <c r="J5" t="str">
         <v>BOOL</v>
       </c>
-      <c r="K4" t="str">
+      <c r="K5" t="str">
         <v>COUNT</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K5"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -719,13 +754,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs5e3pk-ust9</v>
+        <v>lgs8j8fo-0lfw</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T15:41:12.392Z</v>
+        <v>2023-04-22T17:09:10.644Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs5e3pk</v>
+        <v>lgs8j8fo</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -745,13 +780,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs5e3pk-euus</v>
+        <v>lgs8j8fo-s0ps</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T15:41:12.392Z</v>
+        <v>2023-04-22T17:09:10.644Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs5e3pk</v>
+        <v>lgs8j8fo</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -760,10 +795,10 @@
         <v>0m7w</v>
       </c>
       <c r="F3" t="str">
-        <v>lgs5e3pv-5ph5n</v>
+        <v>lgs8j8g0-mpib</v>
       </c>
       <c r="G3" t="str">
-        <v>2023-04-22T10:41:12</v>
+        <v>2023-04-22T12:09:10</v>
       </c>
       <c r="H3" t="str">
         <v/>
@@ -811,13 +846,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs5e3pk-00bg</v>
+        <v>lgs8j8fo-afsz</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T15:41:12.392Z</v>
+        <v>2023-04-22T17:09:10.644Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs5e3pk</v>
+        <v>lgs8j8fo</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -837,13 +872,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs5e3pk-5gq2</v>
+        <v>lgs8j8fo-x1oi</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T15:41:12.392Z</v>
+        <v>2023-04-22T17:09:10.644Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs5e3pk</v>
+        <v>lgs8j8fo</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -870,7 +905,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -894,23 +929,77 @@
       <c r="F1" t="str">
         <v>_lbl</v>
       </c>
-      <c r="G1" t="str">
-        <v>_emoji</v>
-      </c>
-      <c r="H1" t="str">
-        <v>_desc</v>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>lgs8j8g0-063q</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2023-04-22T17:09:10.656Z</v>
+      </c>
+      <c r="C2" t="str">
+        <v>lgs8j8g0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <v>0q9d</v>
+      </c>
+      <c r="F2" t="str">
+        <v>My Tag!</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>lgs8j8g0-r9pi</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2023-04-22T17:09:10.656Z</v>
+      </c>
+      <c r="C3" t="str">
+        <v>lgs8j8g0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
+        <v>vvct</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Orig Tag Label</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>lgs8j8g0-83ol</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2023-04-22T17:09:10.656Z</v>
+      </c>
+      <c r="C4" t="str">
+        <v>lgs8j8g0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
+        <v>0vvi</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Select Option Test</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -938,9 +1027,52 @@
         <v>tid</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>lgs8j8g0-31g6</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2023-04-22T17:09:10.656Z</v>
+      </c>
+      <c r="C2" t="str">
+        <v>lgs8j8g0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <v>ay7l</v>
+      </c>
+      <c r="G2" t="str">
+        <v>vvct</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>lgs8j8g0-uq0p</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2023-04-22T17:09:10.656Z</v>
+      </c>
+      <c r="C3" t="str">
+        <v>lgs8j8g0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
+        <v>0m7w</v>
+      </c>
+      <c r="F3" t="str">
+        <v>8esq</v>
+      </c>
+      <c r="G3" t="str">
+        <v>0vvi</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
can parse from excel too
</commit_message>
<xml_diff>
--- a/data-files/OutExcel1.xlsx
+++ b/data-files/OutExcel1.xlsx
@@ -438,13 +438,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs8j8fo-06px</v>
+        <v>lgsauyu8-4goi</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T17:09:10.644Z</v>
+        <v>2023-04-22T18:14:17.312Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs8j8fo</v>
+        <v>lgsauyu9</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -467,13 +467,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs8j8fo-0oj7</v>
+        <v>lgsauyu9-tbmb</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T17:09:10.644Z</v>
+        <v>2023-04-22T18:14:17.313Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs8j8fo</v>
+        <v>lgsauyu9</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -496,13 +496,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgs8j8fo-03ay</v>
+        <v>lgsauyu9-m24n</v>
       </c>
       <c r="B4" t="str">
-        <v>2023-04-22T17:09:10.644Z</v>
+        <v>2023-04-22T18:14:17.313Z</v>
       </c>
       <c r="C4" t="str">
-        <v>lgs8j8fo</v>
+        <v>lgsauyu9</v>
       </c>
       <c r="D4" t="str">
         <v>FALSE</v>
@@ -574,13 +574,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs8j8fo-pjps</v>
+        <v>lgsauyu9-09r5</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T17:09:10.644Z</v>
+        <v>2023-04-22T18:14:17.313Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs8j8fo</v>
+        <v>lgsauyu9</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -609,13 +609,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs8j8fo-27z6i</v>
+        <v>lgsauyu9-s0u5</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T17:09:10.644Z</v>
+        <v>2023-04-22T18:14:17.313Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs8j8fo</v>
+        <v>lgsauyu9</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -624,7 +624,7 @@
         <v>05a8</v>
       </c>
       <c r="F3" t="str">
-        <v>1vb5</v>
+        <v>0ksk</v>
       </c>
       <c r="G3" t="str">
         <v>Free Item</v>
@@ -644,13 +644,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgs8j8fo-62i6</v>
+        <v>lgsauyu9-v7tg</v>
       </c>
       <c r="B4" t="str">
-        <v>2023-04-22T17:09:10.644Z</v>
+        <v>2023-04-22T18:14:17.313Z</v>
       </c>
       <c r="C4" t="str">
-        <v>lgs8j8fo</v>
+        <v>lgsauyu9</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -679,13 +679,13 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>lgs8j8fo-nljl</v>
+        <v>lgsauyu9-og4k</v>
       </c>
       <c r="B5" t="str">
-        <v>2023-04-22T17:09:10.644Z</v>
+        <v>2023-04-22T18:14:17.313Z</v>
       </c>
       <c r="C5" t="str">
-        <v>lgs8j8fo</v>
+        <v>lgsauyu9</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -754,13 +754,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs8j8fo-0lfw</v>
+        <v>lgsauyu9-p2y4</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T17:09:10.644Z</v>
+        <v>2023-04-22T18:14:17.313Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs8j8fo</v>
+        <v>lgsauyu9</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -780,13 +780,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs8j8fo-s0ps</v>
+        <v>lgsauyu9-3yeb</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T17:09:10.644Z</v>
+        <v>2023-04-22T18:14:17.313Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs8j8fo</v>
+        <v>lgsauyu9</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -795,10 +795,10 @@
         <v>0m7w</v>
       </c>
       <c r="F3" t="str">
-        <v>lgs8j8g0-mpib</v>
+        <v>lgsauyul-0g07</v>
       </c>
       <c r="G3" t="str">
-        <v>2023-04-22T12:09:10</v>
+        <v>2023-04-22T13:14:17</v>
       </c>
       <c r="H3" t="str">
         <v/>
@@ -846,13 +846,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs8j8fo-afsz</v>
+        <v>lgsauyu9-ydzh</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T17:09:10.644Z</v>
+        <v>2023-04-22T18:14:17.313Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs8j8fo</v>
+        <v>lgsauyu9</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -872,13 +872,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs8j8fo-x1oi</v>
+        <v>lgsauyu9-mokn</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T17:09:10.644Z</v>
+        <v>2023-04-22T18:14:17.313Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs8j8fo</v>
+        <v>lgsauyu9</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -932,19 +932,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs8j8g0-063q</v>
+        <v>lgsauyul-xsvg</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T17:09:10.656Z</v>
+        <v>2023-04-22T18:14:17.325Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs8j8g0</v>
+        <v>lgsauyul</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="str">
-        <v>0q9d</v>
+        <v>05c2</v>
       </c>
       <c r="F2" t="str">
         <v>My Tag!</v>
@@ -952,13 +952,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs8j8g0-r9pi</v>
+        <v>lgsauyul-h3kr</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T17:09:10.656Z</v>
+        <v>2023-04-22T18:14:17.325Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs8j8g0</v>
+        <v>lgsauyul</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgs8j8g0-83ol</v>
+        <v>lgsauyul-g8mm</v>
       </c>
       <c r="B4" t="str">
-        <v>2023-04-22T17:09:10.656Z</v>
+        <v>2023-04-22T18:14:17.325Z</v>
       </c>
       <c r="C4" t="str">
-        <v>lgs8j8g0</v>
+        <v>lgsauyul</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1024,18 +1024,18 @@
         <v>_pid</v>
       </c>
       <c r="G1" t="str">
-        <v>tid</v>
+        <v>_tid</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgs8j8g0-31g6</v>
+        <v>lgsauyul-gzp5</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-22T17:09:10.656Z</v>
+        <v>2023-04-22T18:14:17.325Z</v>
       </c>
       <c r="C2" t="str">
-        <v>lgs8j8g0</v>
+        <v>lgsauyul</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -1049,13 +1049,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgs8j8g0-uq0p</v>
+        <v>lgsauyul-0jnx</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-04-22T17:09:10.656Z</v>
+        <v>2023-04-22T18:14:17.325Z</v>
       </c>
       <c r="C3" t="str">
-        <v>lgs8j8g0</v>
+        <v>lgsauyul</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
created from & to tested. Also native excel dates!
</commit_message>
<xml_diff>
--- a/data-files/OutExcel1.xlsx
+++ b/data-files/OutExcel1.xlsx
@@ -418,7 +418,7 @@
         <v>Last updated:</v>
       </c>
       <c r="B2" t="str">
-        <v>4/24/2023, 4:39:40 PM CDT</v>
+        <v>4/24/2023, 9:19:59 PM CDT</v>
       </c>
     </row>
     <row r="3">
@@ -543,13 +543,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgvd2meq-0dvl</v>
+        <v>lgvn3af5-0vhh</v>
       </c>
       <c r="B2" t="str">
-        <v>lgvd2met</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>lgvd2met</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -572,13 +572,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgvd2srg-2iap</v>
+        <v>lgvn3af9-uinj</v>
       </c>
       <c r="B3" t="str">
-        <v>lgvd2srg</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>lgvd2srh</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -601,13 +601,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgvd2srh-p9y5</v>
+        <v>lgvn3af9-iguo</v>
       </c>
       <c r="B4" t="str">
-        <v>lgvd2sri</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C4" t="str">
-        <v>lgvd2sri</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D4" t="str">
         <v>FALSE</v>
@@ -679,13 +679,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgvd2sre-03jg</v>
+        <v>lgvn3af8-wrlz</v>
       </c>
       <c r="B2" t="str">
-        <v>lgvd2sre</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>lgvd2srf</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -714,13 +714,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgvd2srj-0l0p</v>
+        <v>lgvn3afa-3yx8</v>
       </c>
       <c r="B3" t="str">
-        <v>lgvd2srj</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>lgvd2srj</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -729,7 +729,7 @@
         <v>05a8</v>
       </c>
       <c r="F3" t="str">
-        <v>dste</v>
+        <v>4asr</v>
       </c>
       <c r="G3" t="str">
         <v>Free Item</v>
@@ -749,13 +749,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgvd2srk-0kv9</v>
+        <v>lgvn3afa-0sdd</v>
       </c>
       <c r="B4" t="str">
-        <v>lgvd2srk</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C4" t="str">
-        <v>lgvd2srk</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D4" t="str">
         <v>FALSE</v>
@@ -784,13 +784,13 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>lgvd2srl-pb7n</v>
+        <v>lgvn3afb-t5le</v>
       </c>
       <c r="B5" t="str">
-        <v>lgvd2srl</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C5" t="str">
-        <v>lgvd2srl</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D5" t="str">
         <v>FALSE</v>
@@ -826,7 +826,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -856,16 +856,19 @@
       <c r="H1" t="str">
         <v>_note</v>
       </c>
+      <c r="I1" t="str">
+        <v>_source</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgvd2srm-jd3o</v>
+        <v>lgvn3afc-w7is</v>
       </c>
       <c r="B2" t="str">
-        <v>lgvd2srm</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>lgvd2srm</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -882,16 +885,19 @@
       <c r="H2" t="str">
         <v>Orig note</v>
       </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgvd2srp-v8mb</v>
+        <v>lgvn3afd-wyox</v>
       </c>
       <c r="B3" t="str">
-        <v>lgvd2srp</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>lgvd2srq</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -900,18 +906,21 @@
         <v>0m7w</v>
       </c>
       <c r="F3" t="str">
-        <v>lgvd2srr-ginp</v>
+        <v>lgvn3afe-es8h</v>
       </c>
       <c r="G3" t="str">
-        <v>2023-04-24T16:39:40</v>
+        <v>2023-04-24T21:19:59</v>
       </c>
       <c r="H3" t="str">
         <v/>
       </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -951,13 +960,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgvd2sro-0v1h</v>
+        <v>lgvn3afd-5xgh</v>
       </c>
       <c r="B2" t="str">
-        <v>lgvd2sro</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>lgvd2sro</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -977,13 +986,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgvd2sro-0n8o</v>
+        <v>lgvn3afd-jlpc</v>
       </c>
       <c r="B3" t="str">
-        <v>lgvd2srp</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>lgvd2srp</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -1037,19 +1046,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgvd2srr-a2ma</v>
+        <v>lgvn3afe-gxwn</v>
       </c>
       <c r="B2" t="str">
-        <v>lgvd2srr</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>lgvd2srs</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
       </c>
       <c r="E2" t="str">
-        <v>0kcl</v>
+        <v>v0bw</v>
       </c>
       <c r="F2" t="str">
         <v>My Tag!</v>
@@ -1057,13 +1066,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgvd2srs-frdi</v>
+        <v>lgvn3aff-cdea</v>
       </c>
       <c r="B3" t="str">
-        <v>lgvd2srs</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>lgvd2srs</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -1077,13 +1086,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgvd2srt-0ujx</v>
+        <v>lgvn3aff-wulj</v>
       </c>
       <c r="B4" t="str">
-        <v>lgvd2srt</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C4" t="str">
-        <v>lgvd2srt</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D4" t="str">
         <v>FALSE</v>
@@ -1134,13 +1143,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgvd2srv-a6gm</v>
+        <v>lgvn3afg-758d</v>
       </c>
       <c r="B2" t="str">
-        <v>lgvd2srv</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>lgvd2srv</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -1154,13 +1163,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgvd2srw-301n</v>
+        <v>lgvn3afg-rluc</v>
       </c>
       <c r="B3" t="str">
-        <v>lgvd2srw</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>lgvd2srw</v>
+        <v>4/24/2023, 9:19:59 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>

</xml_diff>

<commit_message>
some terrible progress on ExcelNatural
</commit_message>
<xml_diff>
--- a/data-files/OutExcel1.xlsx
+++ b/data-files/OutExcel1.xlsx
@@ -418,7 +418,7 @@
         <v>Last updated:</v>
       </c>
       <c r="B2" t="str">
-        <v>4/25/2023, 10:06:45 PM CDT</v>
+        <v>4/28/2023, 1:46:02 PM CDT</v>
       </c>
     </row>
     <row r="3">
@@ -543,13 +543,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgx47ad1-mkpc</v>
+        <v>lh0wmwkt-vnhp</v>
       </c>
       <c r="B2" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -572,13 +572,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgx47ad4-0rd6</v>
+        <v>lh0wmwkx-0sbz</v>
       </c>
       <c r="B3" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -601,13 +601,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgx47ad5-ukic</v>
+        <v>lh0wmwky-q0sf</v>
       </c>
       <c r="B4" t="str">
         <v>4/24/2023, 8:51:59 PM</v>
       </c>
       <c r="C4" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D4" t="str">
         <v>FALSE</v>
@@ -679,13 +679,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgx47ad3-ssh8</v>
+        <v>lh0wmwkw-xm25</v>
       </c>
       <c r="B2" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -714,13 +714,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgx47ad5-xvt9</v>
+        <v>lh0wmwky-ckzr</v>
       </c>
       <c r="B3" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -729,7 +729,7 @@
         <v>05a8</v>
       </c>
       <c r="F3" t="str">
-        <v>2wcj</v>
+        <v>0f3n</v>
       </c>
       <c r="G3" t="str">
         <v>Free Item</v>
@@ -749,13 +749,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgx47ad6-09rg</v>
+        <v>lh0wmwkz-heaj</v>
       </c>
       <c r="B4" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C4" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D4" t="str">
         <v>FALSE</v>
@@ -776,7 +776,7 @@
         <v>Set a description</v>
       </c>
       <c r="J4" t="str">
-        <v>NUM</v>
+        <v>NUMBER</v>
       </c>
       <c r="K4" t="str">
         <v>AVERAGE</v>
@@ -784,13 +784,13 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>lgx47ad6-0o8a</v>
+        <v>lh0wmwkz-iqss</v>
       </c>
       <c r="B5" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C5" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D5" t="str">
         <v>FALSE</v>
@@ -862,13 +862,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgx47ad7-0ch3</v>
+        <v>lh0wmwl0-zqz7</v>
       </c>
       <c r="B2" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -891,13 +891,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgx47ad9-0pbn</v>
+        <v>lh0wmwl1-y0d3</v>
       </c>
       <c r="B3" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -906,10 +906,10 @@
         <v>0m7w</v>
       </c>
       <c r="F3" t="str">
-        <v>lgx47adb-xuql</v>
+        <v>lh0wmwl2-bkai</v>
       </c>
       <c r="G3" t="str">
-        <v>2023-04-25T22:06:45</v>
+        <v>2023-04-28T13:46:02</v>
       </c>
       <c r="H3" t="str">
         <v/>
@@ -960,13 +960,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgx47ad8-4xkc</v>
+        <v>lh0wmwl1-crrp</v>
       </c>
       <c r="B2" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgx47ad8-8dud</v>
+        <v>lh0wmwl1-07ev</v>
       </c>
       <c r="B3" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -1046,19 +1046,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgx47adb-l2b1</v>
+        <v>lh0wmwl2-036u</v>
       </c>
       <c r="B2" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
       </c>
       <c r="E2" t="str">
-        <v>6775</v>
+        <v>plp7</v>
       </c>
       <c r="F2" t="str">
         <v>My Tag!</v>
@@ -1066,13 +1066,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgx47adb-ollf</v>
+        <v>lh0wmwl3-6xxo</v>
       </c>
       <c r="B3" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -1086,13 +1086,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lgx47adc-pw76</v>
+        <v>lh0wmwl4-0bew</v>
       </c>
       <c r="B4" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C4" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D4" t="str">
         <v>FALSE</v>
@@ -1143,13 +1143,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lgx47adc-svsr</v>
+        <v>lh0wmwl4-1lqh</v>
       </c>
       <c r="B2" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -1163,13 +1163,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lgx47add-vqm8</v>
+        <v>lh0wmwl5-0l5y</v>
       </c>
       <c r="B3" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>4/25/2023, 10:06:45 PM</v>
+        <v>4/28/2023, 1:46:02 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>

</xml_diff>

<commit_message>
about to click go
</commit_message>
<xml_diff>
--- a/data-files/OutExcel1.xlsx
+++ b/data-files/OutExcel1.xlsx
@@ -418,7 +418,7 @@
         <v>Last updated:</v>
       </c>
       <c r="B2" t="str">
-        <v>4/28/2023, 1:46:02 PM CDT</v>
+        <v>4/29/2023, 10:51:20 PM CDT</v>
       </c>
     </row>
     <row r="3">
@@ -481,7 +481,7 @@
         <v>tagDefs</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -492,7 +492,7 @@
         <v>tags</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -543,13 +543,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lh0wmwkt-vnhp</v>
+        <v>lh2vk0q0-0db6</v>
       </c>
       <c r="B2" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -572,13 +572,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lh0wmwkx-0sbz</v>
+        <v>lh2vk0q3-0dtj</v>
       </c>
       <c r="B3" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -601,13 +601,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lh0wmwky-q0sf</v>
+        <v>lh2vk0q4-0a06</v>
       </c>
       <c r="B4" t="str">
         <v>4/24/2023, 8:51:59 PM</v>
       </c>
       <c r="C4" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D4" t="str">
         <v>FALSE</v>
@@ -679,13 +679,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lh0wmwkw-xm25</v>
+        <v>lh2vk0q2-ojke</v>
       </c>
       <c r="B2" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -714,13 +714,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lh0wmwky-ckzr</v>
+        <v>lh2vk0q4-0o48</v>
       </c>
       <c r="B3" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -729,7 +729,7 @@
         <v>05a8</v>
       </c>
       <c r="F3" t="str">
-        <v>0f3n</v>
+        <v>0iu2</v>
       </c>
       <c r="G3" t="str">
         <v>Free Item</v>
@@ -749,13 +749,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lh0wmwkz-heaj</v>
+        <v>lh2vk0q5-klza</v>
       </c>
       <c r="B4" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C4" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D4" t="str">
         <v>FALSE</v>
@@ -784,13 +784,13 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>lh0wmwkz-iqss</v>
+        <v>lh2vk0q5-1wpj</v>
       </c>
       <c r="B5" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C5" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D5" t="str">
         <v>FALSE</v>
@@ -862,13 +862,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lh0wmwl0-zqz7</v>
+        <v>lh2vk0q6-0m06</v>
       </c>
       <c r="B2" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -891,13 +891,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lh0wmwl1-y0d3</v>
+        <v>lh2vk0q7-0kef</v>
       </c>
       <c r="B3" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -906,10 +906,10 @@
         <v>0m7w</v>
       </c>
       <c r="F3" t="str">
-        <v>lh0wmwl2-bkai</v>
+        <v>lh2vk0q8-3am6</v>
       </c>
       <c r="G3" t="str">
-        <v>2023-04-28T13:46:02</v>
+        <v>2023-04-29T22:51:20</v>
       </c>
       <c r="H3" t="str">
         <v/>
@@ -960,13 +960,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lh0wmwl1-crrp</v>
+        <v>lh2vk0q6-idb9</v>
       </c>
       <c r="B2" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -986,13 +986,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lh0wmwl1-07ev</v>
+        <v>lh2vk0q7-r0s5</v>
       </c>
       <c r="B3" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -1019,7 +1019,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1046,19 +1046,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lh0wmwl2-036u</v>
+        <v>lh2vk0q9-0iha</v>
       </c>
       <c r="B2" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
       </c>
       <c r="E2" t="str">
-        <v>plp7</v>
+        <v>0x2q</v>
       </c>
       <c r="F2" t="str">
         <v>My Tag!</v>
@@ -1066,13 +1066,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lh0wmwl3-6xxo</v>
+        <v>lh2vk0q9-5k8p</v>
       </c>
       <c r="B3" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -1086,13 +1086,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>lh0wmwl4-0bew</v>
+        <v>lh2vk0qa-qbib</v>
       </c>
       <c r="B4" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C4" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D4" t="str">
         <v>FALSE</v>
@@ -1101,19 +1101,59 @@
         <v>0vvi</v>
       </c>
       <c r="F4" t="str">
-        <v>Select Option Test</v>
+        <v>Select Option To Delete</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>lh2vk0qa-4x8q</v>
+      </c>
+      <c r="B5" t="str">
+        <v>4/29/2023, 10:51:20 PM</v>
+      </c>
+      <c r="C5" t="str">
+        <v>4/29/2023, 10:51:20 PM</v>
+      </c>
+      <c r="D5" t="str">
+        <v>FALSE</v>
+      </c>
+      <c r="E5" t="str">
+        <v>0vva</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Select Option 1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>lh2vk0qb-gn9e</v>
+      </c>
+      <c r="B6" t="str">
+        <v>4/29/2023, 10:51:20 PM</v>
+      </c>
+      <c r="C6" t="str">
+        <v>4/29/2023, 10:51:20 PM</v>
+      </c>
+      <c r="D6" t="str">
+        <v>FALSE</v>
+      </c>
+      <c r="E6" t="str">
+        <v>0vvb</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Select Option 2</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1143,13 +1183,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lh0wmwl4-1lqh</v>
+        <v>lh2vk0qb-bq3o</v>
       </c>
       <c r="B2" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C2" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
@@ -1163,13 +1203,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lh0wmwl5-0l5y</v>
+        <v>lh2vk0qc-98am</v>
       </c>
       <c r="B3" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="C3" t="str">
-        <v>4/28/2023, 1:46:02 PM</v>
+        <v>4/29/2023, 10:51:20 PM</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
@@ -1184,9 +1224,55 @@
         <v>0vvi</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>lh2vk0qc-qss9</v>
+      </c>
+      <c r="B4" t="str">
+        <v>4/29/2023, 10:51:20 PM</v>
+      </c>
+      <c r="C4" t="str">
+        <v>4/29/2023, 10:51:20 PM</v>
+      </c>
+      <c r="D4" t="str">
+        <v>FALSE</v>
+      </c>
+      <c r="E4" t="str">
+        <v>0m7w</v>
+      </c>
+      <c r="F4" t="str">
+        <v>8esq</v>
+      </c>
+      <c r="G4" t="str">
+        <v>0vva</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>lh2vk0qd-95rs</v>
+      </c>
+      <c r="B5" t="str">
+        <v>4/29/2023, 10:51:20 PM</v>
+      </c>
+      <c r="C5" t="str">
+        <v>4/29/2023, 10:51:20 PM</v>
+      </c>
+      <c r="D5" t="str">
+        <v>FALSE</v>
+      </c>
+      <c r="E5" t="str">
+        <v>0m7w</v>
+      </c>
+      <c r="F5" t="str">
+        <v>8esq</v>
+      </c>
+      <c r="G5" t="str">
+        <v>0vvb</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>